<commit_message>
further update new struct
</commit_message>
<xml_diff>
--- a/excel_results/combined_results.xlsx
+++ b/excel_results/combined_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\DSE\Bigger_is_Better\excel_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7D366F1-5BFA-45D5-9304-629717FF4D22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD42329-F475-469A-8204-E20E612F6C33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" activeTab="1" xr2:uid="{6F5A8ADC-0BBA-479C-8570-84A74105B782}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Take off weight [N]</t>
   </si>
@@ -188,34 +187,47 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Design concept 1</t>
+    <t>Quarter chord sweep [rad]</t>
   </si>
   <si>
-    <t>Design concept 2</t>
+    <t>Zero-lift drag coefficient [-]</t>
   </si>
   <si>
-    <t>Design concept 3</t>
+    <t>HIGH SEMIDD 2E</t>
   </si>
   <si>
-    <t>Design concept 4</t>
+    <t>HIGH DD 2E</t>
   </si>
   <si>
-    <t>Design concept 5</t>
+    <t>LOW SEMIDD 2E</t>
   </si>
   <si>
-    <t>Quarter chord sweep [rad]</t>
+    <t>HIGH DD 2E STRUT</t>
+  </si>
+  <si>
+    <t>HIGH SEMIDD 2E STRUT</t>
+  </si>
+  <si>
+    <t>Landing gear weight [N]</t>
+  </si>
+  <si>
+    <t>W/S [N/m^2]</t>
+  </si>
+  <si>
+    <t>T/w [-]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +245,13 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -319,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -330,8 +349,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -349,6 +366,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -9318,8 +9338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2871581C-8947-4279-9BF5-986AB6A255DE}">
   <dimension ref="A1:CV2735"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9356,288 +9376,288 @@
     <col min="100" max="100" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:82" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="B1" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="28" t="s">
         <v>55</v>
       </c>
+      <c r="E1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:82" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="18">
         <v>1580051.3060698099</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="19">
         <v>1520114.4389424899</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="18">
         <v>1597097.40303844</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="19">
         <v>1532733.6181717799</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="18">
         <v>1474914.2672244101</v>
       </c>
     </row>
     <row r="3" spans="1:82" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="18">
         <v>472485.24524999998</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>472485.24524999998</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <v>472485.24524999998</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="19">
         <v>472485.24524999998</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="18">
         <v>472485.24524999998</v>
       </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="18">
         <v>141375.518052842</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <v>136151.86323993001</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="18">
         <v>142824.683749816</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <v>137159.42504139201</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="18">
         <v>131089.07847274601</v>
       </c>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="18">
         <v>966190.54276697105</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="19">
         <v>911477.33045256895</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="18">
         <v>981787.474038632</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>923088.94788038905</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="18">
         <v>871339.94350167201</v>
       </c>
     </row>
     <row r="6" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <v>214922.15532104301</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="19">
         <v>208030.913446405</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <v>222815.35528357999</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>212271.98633827601</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="18">
         <v>137586.79017798501</v>
       </c>
     </row>
     <row r="7" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="18">
         <v>20916.9344340469</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="19">
         <v>19366.3440218346</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="18">
         <v>19596.413771753501</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>34042.894860766501</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="18">
         <v>16381.0027715162</v>
       </c>
     </row>
     <row r="8" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <v>244231.168107957</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="19">
         <v>209884.50072030199</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <v>248720.80338146401</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
         <v>206842.94002626301</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="18">
         <v>246937.263629383</v>
       </c>
     </row>
     <row r="9" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="18">
         <v>27753.271561695699</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="19">
         <v>28707.6603054484</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="18">
         <v>30114.6264674866</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>22936.635005443401</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="18">
         <v>27640.1706520767</v>
       </c>
     </row>
     <row r="10" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="18">
         <v>126254.55726617599</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="19">
         <v>126187.53070403299</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="18">
         <v>126249.70425092999</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <v>126282.34702421</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="18">
         <v>126200.83276709</v>
       </c>
     </row>
     <row r="11" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="18">
         <v>293675.049641572</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="19">
         <v>282059.53383109201</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="18">
         <v>295522.473491907</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>283239.936021681</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="18">
         <v>280519.77486059198</v>
       </c>
     </row>
     <row r="12" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>0.697994414465406</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>0.56975049023278201</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <v>0.69726809353464103</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="11">
         <v>0.62918857331470801</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>0.622110056992491</v>
       </c>
     </row>
     <row r="13" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>3.7449999999999997E-2</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>3.3259999999999998E-2</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <v>3.8159999999999999E-2</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <v>3.1029999999999999E-2</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <v>3.6240000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>18.638035099209699</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>17.130201149512299</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <v>18.272224673339601</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="11">
         <v>20.276782897670198</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>17.166392301117298</v>
       </c>
     </row>
     <row r="15" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="9">
@@ -9728,7 +9748,7 @@
       <c r="CD15" s="3"/>
     </row>
     <row r="16" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="8">
@@ -9748,7 +9768,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="8">
@@ -9768,287 +9788,287 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <v>210.85106599578799</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="17">
         <v>190.36910016875601</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <v>199.69911450587901</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="17">
         <v>255.70384621453101</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="16">
         <v>183.29025631350601</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>52.355170307671202</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="17">
         <v>49.747344674804701</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>50.951825174143003</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <v>61.931879458143101</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="16">
         <v>50.656328216611598</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>6.1516127777055098</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="17">
         <v>5.8451992298000297</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="16">
         <v>6.04218540712652</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="17">
         <v>6.3650329322472103</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="16">
         <v>5.5268596659399396</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="16">
         <v>1.9030288080900499</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="17">
         <v>1.8082384124776201</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="16">
         <v>1.7965569273570099</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="17">
         <v>1.89255099550519</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <v>1.70975865071886</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="18">
+      <c r="A22" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="16">
         <v>0.45322773323204502</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="17">
         <v>0.45322773323204502</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <v>0.51332191392368598</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="17">
         <v>0.51332191392368598</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <v>0.45322773323204502</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="16">
         <v>0.30935445335359002</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="17">
         <v>0.30935445335359002</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="16">
         <v>0.29733561721526203</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="17">
         <v>0.29733561721526203</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <v>0.30935445335359002</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="16">
         <v>53.998516569010597</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="17">
         <v>50.422636868395202</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="16">
         <v>53.998516569010597</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="17">
         <v>50.422636868395202</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="16">
         <v>53.998516569010597</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="16">
         <v>6.2877186341350804</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="17">
         <v>5.9507847046706299</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="16">
         <v>6.2877186341350804</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="17">
         <v>5.9507847046706299</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <v>6.2877186341350804</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>11.6322794731499</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="17">
         <v>11.0089517036406</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="16">
         <v>11.6322794731499</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="17">
         <v>11.0089517036406</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="16">
         <v>11.6322794731499</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <v>20.7494714926457</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="17">
         <v>19.637589525413102</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="16">
         <v>20.7494714926457</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="17">
         <v>19.637589525413102</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="16">
         <v>20.7494714926457</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="16">
         <v>28.910976055334501</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="17">
         <v>26.913827234038401</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="16">
         <v>29.016455845168501</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="17">
         <v>26.227753049629499</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="16">
         <v>29.133929444647801</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="16">
         <v>31.776773710913002</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="17">
         <v>29.283951349043399</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="16">
         <v>29.317448869129102</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="17">
         <v>43.751768464589901</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="16">
         <v>24.627513095698902</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="16">
         <v>29.9970534087016</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="17">
         <v>27.617694577759</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="16">
         <v>27.583785442710901</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="17">
         <v>47.053606684339002</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="16">
         <v>25.139915722426601</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="18">
         <v>426973.40864147199</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="19">
         <v>441656.31239151402</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="18">
         <v>463301.94565364101</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="19">
         <v>352871.30777605303</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="18">
         <v>425233.394647334</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="8">
@@ -10068,27 +10088,27 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="16">
         <v>224.576689295661</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="17">
         <v>229.43040611479501</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="16">
         <v>232.06257893885001</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="17">
         <v>228.65779722382001</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="16">
         <v>227.82399045096099</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="8">
@@ -10108,120 +10128,241 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="12">
         <v>8.1351725770621598E-3</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="13">
         <v>8.4710380578120002E-3</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="12">
         <v>8.3830977597687695E-3</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="13">
         <v>7.2094496184857398E-3</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="12">
         <v>8.1899295050168394E-3</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="16">
+      <c r="B36" s="14">
         <v>13.4556108823174</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="15">
         <v>9.8825738530638301</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="14">
         <v>10.818108938629999</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="15">
         <v>23.3037274629175</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="14">
         <v>12.873090372161199</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="14">
         <v>24.283709451511498</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="15">
         <v>29.614074304697599</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="14">
         <v>21.9762015295493</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="15">
         <v>28.101697657103198</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="14">
         <v>29.224562289017399</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="24">
+      <c r="B38" s="22">
         <v>10.397479204424799</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="23">
         <v>10.707349053201099</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="22">
         <v>11.9942466975647</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="23">
         <v>15.8039258708273</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="22">
         <v>11.336181647266001</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A39" s="22"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
-      <c r="B40" s="6">
+      <c r="A40" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="27">
         <f>B13-(B12^2)/(PI()*B17*B16)</f>
         <v>2.3415668071791081E-2</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="27">
         <f>C13-(C12^2)/(PI()*C17*C16)</f>
         <v>2.3909017066756071E-2</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="27">
         <f>D13-(D12^2)/(PI()*D17*D16)</f>
         <v>2.4154860642002351E-2</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="27">
         <f>E13-(E12^2)/(PI()*E17*E16)</f>
         <v>2.1146708695322546E-2</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="27">
         <f>F13-(F12^2)/(PI()*F17*F16)</f>
         <v>2.5887681852567998E-2</v>
       </c>
       <c r="Y40"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B41" s="23"/>
+      <c r="B41" s="21"/>
       <c r="Y41"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B42" s="19">
+        <f>SUM(B6:B11)</f>
+        <v>927753.13633249071</v>
+      </c>
+      <c r="C42" s="19">
+        <f t="shared" ref="C42:F42" si="0">SUM(C6:C11)</f>
+        <v>874236.48302911501</v>
+      </c>
+      <c r="D42" s="19">
+        <f t="shared" si="0"/>
+        <v>943019.37664712116</v>
+      </c>
+      <c r="E42" s="19">
+        <f t="shared" si="0"/>
+        <v>885616.73927663988</v>
+      </c>
+      <c r="F42" s="19">
+        <f t="shared" si="0"/>
+        <v>835265.83485864289</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="19">
+        <f>B5-B42</f>
+        <v>38437.406434480334</v>
+      </c>
+      <c r="C43" s="19">
+        <f t="shared" ref="C43:F43" si="1">C5-C42</f>
+        <v>37240.847423453932</v>
+      </c>
+      <c r="D43" s="19">
+        <f t="shared" si="1"/>
+        <v>38768.097391510848</v>
+      </c>
+      <c r="E43" s="19">
+        <f t="shared" si="1"/>
+        <v>37472.208603749168</v>
+      </c>
+      <c r="F43" s="19">
+        <f t="shared" si="1"/>
+        <v>36074.108643029118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="6">
+        <f>B2/B18</f>
+        <v>7493.6842202228818</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" ref="C45:F45" si="2">C2/C18</f>
+        <v>7985.0902147195002</v>
+      </c>
+      <c r="D45" s="6">
+        <f t="shared" si="2"/>
+        <v>7997.518702024202</v>
+      </c>
+      <c r="E45" s="6">
+        <f t="shared" si="2"/>
+        <v>5994.1750617464058</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="2"/>
+        <v>8046.8776512684099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="6">
+        <f>B31/B2</f>
+        <v>0.27022755970090467</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" ref="C46:F46" si="3">C31/C2</f>
+        <v>0.29054148890182541</v>
+      </c>
+      <c r="D46" s="6">
+        <f t="shared" si="3"/>
+        <v>0.29008997495845901</v>
+      </c>
+      <c r="E46" s="6">
+        <f t="shared" si="3"/>
+        <v>0.23022350628477262</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" si="3"/>
+        <v>0.28831058461965114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B48" s="6">
+        <f>B4/B2</f>
+        <v>8.9475270524282419E-2</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" ref="C48:F48" si="4">C4/C2</f>
+        <v>8.9566850858049774E-2</v>
+      </c>
+      <c r="D48" s="6">
+        <f t="shared" si="4"/>
+        <v>8.9427660127738867E-2</v>
+      </c>
+      <c r="E48" s="6">
+        <f t="shared" si="4"/>
+        <v>8.9486798890073008E-2</v>
+      </c>
+      <c r="F48" s="6">
+        <f t="shared" si="4"/>
+        <v>8.8879117509275976E-2</v>
+      </c>
     </row>
     <row r="49" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>

</xml_diff>